<commit_message>
Mudanças no gravar o ficheiro e começo do random Forest
</commit_message>
<xml_diff>
--- a/Projeto/Results/Logistic_Regression.xlsx
+++ b/Projeto/Results/Logistic_Regression.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,18 +453,18 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>16018</v>
+        <v>16020</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>19092</v>
+        <v>19093</v>
       </c>
     </row>
     <row r="9">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.9998291377150017</v>
+        <v>0.9999145688575009</v>
       </c>
     </row>
     <row r="37">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.9997905320485966</v>
+        <v>0.9998952605394082</v>
       </c>
     </row>
     <row r="41">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.9998952550539436</v>
+        <v>0.9999476275269719</v>
       </c>
     </row>
     <row r="45">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.9998428908091124</v>
+        <v>0.9999214433475608</v>
       </c>
     </row>
     <row r="49">
@@ -671,8 +671,49 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>0:01:26.229654</t>
-        </is>
+          <t>0:01:28.510974</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Melhores Parâmetros</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>solver</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>liblinear</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>penalty</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes na análise, markdown e readme
</commit_message>
<xml_diff>
--- a/Projeto/Results/Logistic_Regression.xlsx
+++ b/Projeto/Results/Logistic_Regression.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -461,10 +461,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>19094</v>
+        <v>19093</v>
       </c>
     </row>
     <row r="11">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.9999715229525002</v>
+        <v>0.9999430459050006</v>
       </c>
     </row>
     <row r="37">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.9999476302697041</v>
+        <v>0.9999476275269719</v>
       </c>
     </row>
     <row r="41">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>0.9999476275269719</v>
       </c>
     </row>
     <row r="45">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.999973814449187</v>
+        <v>0.9999476275269719</v>
       </c>
     </row>
     <row r="49">
@@ -671,7 +671,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>0:01:21.781927</t>
+          <t>0:05:21.054732</t>
         </is>
       </c>
     </row>

</xml_diff>